<commit_message>
Table Atan sur 64 bits Correction d'un problème de perte de précision de l'algo CoRDiC
</commit_message>
<xml_diff>
--- a/Documentation/Feuille de calcul CoRDiC.xlsx
+++ b/Documentation/Feuille de calcul CoRDiC.xlsx
@@ -8,15 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Cosinus &amp; Sinus" sheetId="3" r:id="rId1"/>
-    <sheet name="Angle &amp; Magnitude" sheetId="4" r:id="rId2"/>
-    <sheet name="Steps" sheetId="7" r:id="rId3"/>
+    <sheet name="Cosinus &amp; Sinus (2)" sheetId="9" r:id="rId2"/>
+    <sheet name="Angle &amp; Magnitude" sheetId="4" r:id="rId3"/>
+    <sheet name="Steps" sheetId="7" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>i</t>
   </si>
@@ -74,7 +76,7 @@
     <numFmt numFmtId="164" formatCode="0.000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +88,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,6 +130,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,14 +431,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
@@ -440,11 +454,11 @@
         <v>6</v>
       </c>
       <c r="B1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>DEC2HEX(B1/180*PI()*POWER(2,15),4)</f>
-        <v>C90F</v>
+        <v>0000</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -452,11 +466,12 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <f>-1/128</f>
+        <v>-7.8125E-3</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>DEC2HEX(B2*POWER(2,15),4)</f>
-        <v>8000</v>
+        <v>FFFFFFFF00</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -467,6 +482,7 @@
         <f>PRODUCT(D7:D22)</f>
         <v>1.6467602578654548</v>
       </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="5" spans="1:12">
       <c r="F5" s="1" t="s">
@@ -522,12 +538,12 @@
         <v>1.4142135623730951</v>
       </c>
       <c r="F7" s="3">
-        <f>B2/B3</f>
-        <v>0.60725293510313938</v>
+        <f>B2</f>
+        <v>-7.8125E-3</v>
       </c>
       <c r="G7" s="3" t="str">
         <f>DEC2HEX(F7*POWER(2,15),4)</f>
-        <v>4DBA</v>
+        <v>FFFFFFFF00</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -538,11 +554,11 @@
       </c>
       <c r="J7" s="3">
         <f>B1</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="K7" s="3" t="str">
         <f>DEC2HEX(INT(J7/360*POWER(2,32)),8)</f>
-        <v>40000000</v>
+        <v>00000000</v>
       </c>
       <c r="L7">
         <f>IF(J7&gt;=0,-1,1)</f>
@@ -567,31 +583,31 @@
       </c>
       <c r="F8" s="3">
         <f>F7+(L7*H7/(2^A7))</f>
-        <v>0.60725293510313938</v>
+        <v>-7.8125E-3</v>
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" ref="G8:G38" si="3">DEC2HEX(F8*POWER(2,15),4)</f>
-        <v>4DBA</v>
+        <v>FFFFFFFF00</v>
       </c>
       <c r="H8" s="3">
         <f>H7-(L7*F7/(2^A7))</f>
-        <v>0.60725293510313938</v>
+        <v>-7.8125E-3</v>
       </c>
       <c r="I8" s="3" t="str">
         <f t="shared" ref="I8:I38" si="4">DEC2HEX(H8*POWER(2,15),4)</f>
-        <v>4DBA</v>
+        <v>FFFFFFFF00</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ref="J8:J22" si="5">J7+B7*L7</f>
-        <v>45</v>
+        <v>-45</v>
       </c>
       <c r="K8" s="3" t="str">
         <f t="shared" ref="K8:K22" si="6">DEC2HEX(INT(J8/360*POWER(2,32)),8)</f>
-        <v>20000000</v>
+        <v>FFE0000000</v>
       </c>
       <c r="L8">
         <f t="shared" ref="L8:L22" si="7">IF(J8&gt;=0,-1,1)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -612,31 +628,31 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ref="F9:F22" si="8">F8+(L8*H8/(2^A8))</f>
-        <v>0.30362646755156969</v>
+        <v>-1.171875E-2</v>
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>26DD</v>
+        <v>FFFFFFFE80</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" ref="H9:H22" si="9">H8-(L8*F8/(2^A8))</f>
-        <v>0.91087940265470912</v>
+        <v>-3.90625E-3</v>
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7497</v>
+        <v>FFFFFFFF80</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="5"/>
-        <v>18.43494882292201</v>
+        <v>-18.43494882292201</v>
       </c>
       <c r="K9" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0D1BFAE2</v>
+        <v>FFF2E4051D</v>
       </c>
       <c r="L9">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -657,31 +673,31 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" si="8"/>
-        <v>7.5906616887892409E-2</v>
+        <v>-1.26953125E-2</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>09B7</v>
+        <v>FFFFFFFE60</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="9"/>
-        <v>0.98678601954260159</v>
+        <v>-9.765625E-4</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7E4F</v>
+        <v>FFFFFFFFE0</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="5"/>
-        <v>4.3987053549955313</v>
+        <v>-4.3987053549955313</v>
       </c>
       <c r="K10" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0320C287</v>
+        <v>FFFCDF3D78</v>
       </c>
       <c r="L10">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -702,31 +718,31 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" si="8"/>
-        <v>-4.744163555493279E-2</v>
+        <v>-1.28173828125E-2</v>
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFF9EE</v>
+        <v>FFFFFFFE5C</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="9"/>
-        <v>0.99627434665358816</v>
+        <v>6.103515625E-4</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7F85</v>
+        <v>0014</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="5"/>
-        <v>-2.7263109939062664</v>
+        <v>2.7263109939062664</v>
       </c>
       <c r="K11" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>FFFE0FB0B2</v>
+        <v>01F04F4D</v>
       </c>
       <c r="L11">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -747,31 +763,31 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" si="8"/>
-        <v>1.482551111091647E-2</v>
+        <v>-1.285552978515625E-2</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>01E5</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="9"/>
-        <v>0.99923944887577143</v>
+        <v>-1.9073486328125E-4</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FE7</v>
+        <v>FFFFFFFFFA</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="5"/>
-        <v>0.85002338109108466</v>
+        <v>-0.85002338109108466</v>
       </c>
       <c r="K12" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>009ABDF5</v>
+        <v>FFFF65420A</v>
       </c>
       <c r="L12">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -792,31 +808,31 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" si="8"/>
-        <v>-1.6400721666451387E-2</v>
+        <v>-1.2861490249633789E-2</v>
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFFDE7</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="9"/>
-        <v>0.99970274609798759</v>
+        <v>2.1100044250488281E-4</v>
       </c>
       <c r="I13" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FF6</v>
+        <v>0006</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="5"/>
-        <v>-0.93988722715498474</v>
+        <v>0.93988722715498474</v>
       </c>
       <c r="K13" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>FFFF54E614</v>
+        <v>00AB19EB</v>
       </c>
       <c r="L13">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -837,31 +853,31 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="8"/>
-        <v>-7.8036625867033103E-4</v>
+        <v>-1.2864787131547928E-2</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFFFE7</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="9"/>
-        <v>0.99995900737402588</v>
+        <v>1.0039657354354858E-5</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFE</v>
+        <v>0000</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="5"/>
-        <v>-4.4713516943910347E-2</v>
+        <v>4.4713516943910347E-2</v>
       </c>
       <c r="K14" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>FFFFF7DC32</v>
+        <v>000823CD</v>
       </c>
       <c r="L14">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -882,31 +898,31 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="8"/>
-        <v>7.0318134864392461E-3</v>
+        <v>-1.2864865566371009E-2</v>
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>00E6</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="9"/>
-        <v>0.99996510398542171</v>
+        <v>-9.0466492110863328E-5</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFE</v>
+        <v>FFFFFFFFFE</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="5"/>
-        <v>0.40290065391664276</v>
+        <v>-0.40290065391664276</v>
       </c>
       <c r="K15" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>00495888</v>
+        <v>FFFFB6A777</v>
       </c>
       <c r="L15">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -927,31 +943,31 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="8"/>
-        <v>3.1256997989961926E-3</v>
+        <v>-1.2865218951105817E-2</v>
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0066</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="9"/>
-        <v>0.9999925720068531</v>
+        <v>-4.0213110992226575E-5</v>
       </c>
       <c r="I16" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>FFFFFFFFFF</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="5"/>
-        <v>0.17909015354810467</v>
+        <v>-0.17909015354810467</v>
       </c>
       <c r="K16" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>00209A34</v>
+        <v>FFFFDF65CB</v>
       </c>
       <c r="L16">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -972,31 +988,31 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="8"/>
-        <v>1.1725893067953076E-3</v>
+        <v>-1.2865297492338224E-2</v>
       </c>
       <c r="G17" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0026</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="9"/>
-        <v>0.99999867688927302</v>
+        <v>-1.5085730228348027E-5</v>
       </c>
       <c r="I17" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="5"/>
-        <v>6.7184476481897779E-2</v>
+        <v>-6.7184476481897779E-2</v>
       </c>
       <c r="K17" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>000C3B06</v>
+        <v>FFFFF3C4F9</v>
       </c>
       <c r="L17">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1017,31 +1033,31 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" si="8"/>
-        <v>1.9602809889562693E-4</v>
+        <v>-1.2865312224496649E-2</v>
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0006</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="9"/>
-        <v>0.99999982199601789</v>
+        <v>-2.5219631459864802E-6</v>
       </c>
       <c r="I18" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="5"/>
-        <v>1.1231584588094104E-2</v>
+        <v>-1.1231584588094104E-2</v>
       </c>
       <c r="K18" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>00020B6E</v>
+        <v>FFFFFDF491</v>
       </c>
       <c r="L18">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1062,31 +1078,31 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" si="8"/>
-        <v>-2.9225306418836618E-4</v>
+        <v>-1.2865313455923967E-2</v>
       </c>
       <c r="G19" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFFFF7</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="9"/>
-        <v>0.99999991771286301</v>
+        <v>3.7599275886310242E-6</v>
       </c>
       <c r="I19" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" si="5"/>
-        <v>-1.6744868028909572E-2</v>
+        <v>1.6744868028909572E-2</v>
       </c>
       <c r="K19" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>FFFFFCF3A1</v>
+        <v>00030C5E</v>
       </c>
       <c r="L19">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1107,31 +1123,31 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" si="8"/>
-        <v>-4.8112459277999234E-5</v>
+        <v>-1.2865314373875038E-2</v>
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>FFFFFFFFFF</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H20" s="3">
         <f t="shared" si="9"/>
-        <v>0.99999998906370879</v>
+        <v>6.1898192068083701E-7</v>
       </c>
       <c r="I20" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" si="5"/>
-        <v>-2.7566408866445558E-3</v>
+        <v>2.7566408866445558E-3</v>
       </c>
       <c r="K20" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>FFFFFF7F87</v>
+        <v>00008078</v>
       </c>
       <c r="L20">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1152,31 +1168,31 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" si="8"/>
-        <v>7.3957851887004281E-5</v>
+        <v>-1.2865314449434354E-2</v>
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0002</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="9"/>
-        <v>0.99999999493681169</v>
+        <v>-9.5149102534883068E-7</v>
       </c>
       <c r="I21" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" si="5"/>
-        <v>4.2374727887083633E-3</v>
+        <v>-4.2374727887083633E-3</v>
       </c>
       <c r="K21" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0000C57B</v>
+        <v>FFFFFF3A84</v>
       </c>
       <c r="L21">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1197,31 +1213,31 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" si="8"/>
-        <v>1.2922695946036771E-5</v>
+        <v>-1.2865314507508756E-2</v>
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="9"/>
-        <v>0.99999999945084073</v>
+        <v>-1.6625454772222219E-7</v>
       </c>
       <c r="I22" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" si="5"/>
-        <v>7.4041593800435249E-4</v>
+        <v>-7.4041593800435249E-4</v>
       </c>
       <c r="K22" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>00002281</v>
+        <v>FFFFFFDD7E</v>
       </c>
       <c r="L22">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1242,31 +1258,31 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" ref="F23:F38" si="10">F22+(L22*H22/(2^A22))</f>
-        <v>-1.7594882162204218E-5</v>
+        <v>-1.2865314512582443E-2</v>
       </c>
       <c r="G23" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" ref="H23:H38" si="11">H22-(L22*F22/(2^A22))</f>
-        <v>0.99999999984521015</v>
+        <v>2.2636369286337218E-7</v>
       </c>
       <c r="I23" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>7FFF</v>
+        <v>0000</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" ref="J23:J38" si="12">J22+B22*L22</f>
-        <v>-1.0081124889760971E-3</v>
+        <v>1.0081124889760971E-3</v>
       </c>
       <c r="K23" s="3" t="str">
         <f t="shared" ref="K23:K38" si="13">DEC2HEX(INT(J23/360*POWER(2,32)),8)</f>
-        <v>FFFFFFD104</v>
+        <v>00002EFB</v>
       </c>
       <c r="L23">
         <f t="shared" ref="L23:L38" si="14">IF(J23&gt;=0,-1,1)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1287,31 +1303,31 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" si="10"/>
-        <v>-2.3360931020661238E-6</v>
+        <v>-1.2865314516036478E-2</v>
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001136868</v>
+        <v>3.0054572493156686E-8</v>
       </c>
       <c r="I24" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="12"/>
-        <v>-1.338482752823168E-4</v>
+        <v>1.338482752823168E-4</v>
       </c>
       <c r="K24" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFF9C3</v>
+        <v>0000063C</v>
       </c>
       <c r="L24">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1332,31 +1348,31 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" si="10"/>
-        <v>5.293301430051238E-6</v>
+        <v>-1.2865314516265776E-2</v>
       </c>
       <c r="G25" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001315099</v>
+        <v>-6.8099987718303262E-8</v>
       </c>
       <c r="I25" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" si="12"/>
-        <v>3.0328383159001777E-4</v>
+        <v>-3.0328383159001777E-4</v>
       </c>
       <c r="K25" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>00000E22</v>
+        <v>FFFFFFF1DD</v>
       </c>
       <c r="L25">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1377,31 +1393,31 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" si="10"/>
-        <v>1.4786041639245675E-6</v>
+        <v>-1.2865314516525556E-2</v>
       </c>
       <c r="G26" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H26" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001517022</v>
+        <v>-1.9022707611698588E-8</v>
       </c>
       <c r="I26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" si="12"/>
-        <v>8.4717778150669926E-5</v>
+        <v>-8.4717778150669926E-5</v>
       </c>
       <c r="K26" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>000003F2</v>
+        <v>FFFFFFFC0D</v>
       </c>
       <c r="L26">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1422,31 +1438,31 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" si="10"/>
-        <v>-4.2874446917728153E-7</v>
+        <v>-1.2865314516561839E-2</v>
       </c>
       <c r="G27" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001545224</v>
+        <v>5.515932442099241E-9</v>
       </c>
       <c r="I27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="12"/>
-        <v>-2.4565248569401559E-5</v>
+        <v>2.4565248569401559E-5</v>
       </c>
       <c r="K27" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFFEDA</v>
+        <v>00000125</v>
       </c>
       <c r="L27">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1467,31 +1483,31 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" si="10"/>
-        <v>5.2492984737633251E-7</v>
+        <v>-1.2865314516567099E-2</v>
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001549312</v>
+        <v>-6.7533875848342759E-9</v>
       </c>
       <c r="I28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="12"/>
-        <v>3.0076264790683881E-5</v>
+        <v>-3.0076264790683881E-5</v>
       </c>
       <c r="K28" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>00000166</v>
+        <v>FFFFFFFE99</v>
       </c>
       <c r="L28">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1512,31 +1528,31 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" si="10"/>
-        <v>4.8092689099330564E-8</v>
+        <v>-1.2865314516570319E-2</v>
       </c>
       <c r="G29" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001551814</v>
+        <v>-6.1872757136500944E-10</v>
       </c>
       <c r="I29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="12"/>
-        <v>2.755508110634947E-6</v>
+        <v>-2.755508110634947E-6</v>
       </c>
       <c r="K29" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>00000020</v>
+        <v>FFFFFFFFDF</v>
       </c>
       <c r="L29">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1557,31 +1573,31 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" si="10"/>
-        <v>-1.9032589003923007E-7</v>
+        <v>-1.2865314516570466E-2</v>
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H30" s="3">
         <f t="shared" si="11"/>
-        <v>1.000000000155193</v>
+        <v>2.4486024353703914E-9</v>
       </c>
       <c r="I30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="12"/>
-        <v>-1.0904870229390296E-5</v>
+        <v>1.0904870229390296E-5</v>
       </c>
       <c r="K30" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFFF7D</v>
+        <v>00000082</v>
       </c>
       <c r="L30">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1602,31 +1618,31 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" si="10"/>
-        <v>-7.1116600469948377E-8</v>
+        <v>-1.2865314516570758E-2</v>
       </c>
       <c r="G31" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H31" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552156</v>
+        <v>9.1493743200267341E-10</v>
       </c>
       <c r="I31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="12"/>
-        <v>-4.0746810593775769E-6</v>
+        <v>4.0746810593775769E-6</v>
       </c>
       <c r="K31" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFFFCF</v>
+        <v>00000030</v>
       </c>
       <c r="L31">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1647,31 +1663,31 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" si="10"/>
-        <v>-1.151195568530618E-8</v>
+        <v>-1.2865314516570811E-2</v>
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H32" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552198</v>
+        <v>1.4810493031879704E-10</v>
       </c>
       <c r="I32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="12"/>
-        <v>-6.5958647437120569E-7</v>
+        <v>6.5958647437120569E-7</v>
       </c>
       <c r="K32" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFFFF8</v>
+        <v>00000007</v>
       </c>
       <c r="L32">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1692,31 +1708,31 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" si="10"/>
-        <v>1.8290366707015044E-8</v>
+        <v>-1.2865314516570817E-2</v>
       </c>
       <c r="G33" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H33" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552203</v>
+        <v>-2.3531132052314275E-10</v>
       </c>
       <c r="I33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" si="12"/>
-        <v>1.0479608181319814E-6</v>
+        <v>-1.0479608181319814E-6</v>
       </c>
       <c r="K33" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>0000000C</v>
+        <v>FFFFFFFFF3</v>
       </c>
       <c r="L33">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1737,31 +1753,31 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" si="10"/>
-        <v>3.3892055108544252E-9</v>
+        <v>-1.286531451657082E-2</v>
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H34" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552205</v>
+        <v>-4.360319510217278E-11</v>
       </c>
       <c r="I34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" si="12"/>
-        <v>1.9418717188038765E-7</v>
+        <v>-1.9418717188038765E-7</v>
       </c>
       <c r="K34" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>00000002</v>
+        <v>FFFFFFFFFD</v>
       </c>
       <c r="L34">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1782,31 +1798,31 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" si="10"/>
-        <v>-4.0613750872258858E-9</v>
+        <v>-1.286531451657082E-2</v>
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H35" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552205</v>
+        <v>5.2250867608312232E-11</v>
       </c>
       <c r="I35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" si="12"/>
-        <v>-2.3269965124540928E-7</v>
+        <v>2.3269965124540928E-7</v>
       </c>
       <c r="K35" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFFFFD</v>
+        <v>00000002</v>
       </c>
       <c r="L35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1827,31 +1843,31 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" si="10"/>
-        <v>-3.3608478818573026E-10</v>
+        <v>-1.286531451657082E-2</v>
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H36" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552205</v>
+        <v>4.323836253069726E-12</v>
       </c>
       <c r="I36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="12"/>
-        <v>-1.9256239682510817E-8</v>
+        <v>1.9256239682510817E-8</v>
       </c>
       <c r="K36" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>FFFFFFFFFF</v>
+        <v>00000000</v>
       </c>
       <c r="L36">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1872,31 +1888,31 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" si="10"/>
-        <v>1.5265603613343475E-9</v>
+        <v>-1.286531451657082E-2</v>
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H37" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552205</v>
+        <v>-1.9639679424551527E-11</v>
       </c>
       <c r="I37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J37" s="3">
         <f t="shared" si="12"/>
-        <v>8.7465466098938417E-8</v>
+        <v>-8.7465466098938417E-8</v>
       </c>
       <c r="K37" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>00000001</v>
+        <v>FFFFFFFFFE</v>
       </c>
       <c r="L37">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1917,31 +1933,31 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" si="10"/>
-        <v>5.9523778657430861E-10</v>
+        <v>-1.286531451657082E-2</v>
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>FFFFFFFE5B</v>
       </c>
       <c r="H38" s="3">
         <f t="shared" si="11"/>
-        <v>1.0000000001552205</v>
+        <v>-7.6579215857409005E-12</v>
       </c>
       <c r="I38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>8000</v>
+        <v>0000</v>
       </c>
       <c r="J38" s="3">
         <f t="shared" si="12"/>
-        <v>3.41046132082138E-8</v>
+        <v>-3.41046132082138E-8</v>
       </c>
       <c r="K38" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>00000000</v>
+        <v>FFFFFFFFFF</v>
       </c>
       <c r="L38">
         <f t="shared" si="14"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1952,9 +1968,1680 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <f>DEC2HEX(B1/180*PI()*POWER(2,15),4)</f>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>-1/128</f>
+        <v>-7.8125E-3</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2*POWER(2,15)</f>
+        <v>-256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>PRODUCT(D7:D22)</f>
+        <v>1.6467602578654548</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <f>DEGREES(ATAN(2^-A7))</f>
+        <v>45</v>
+      </c>
+      <c r="C7" s="6">
+        <f>INT(B7/360*POWER(2,32))</f>
+        <v>536870912</v>
+      </c>
+      <c r="D7" s="3">
+        <f>SQRT(1+POWER(2, -2*A7))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="F7" s="3">
+        <f>C2</f>
+        <v>-256</v>
+      </c>
+      <c r="G7" s="3" t="str">
+        <f>DEC2HEX(F7,8)</f>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f>DEC2HEX(F7/$B$3,8)</f>
+        <v>FFFFFFFF65</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <f>DEC2HEX(I7,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="K7" s="3" t="str">
+        <f>DEC2HEX(I7/$B$3,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="L7" s="6">
+        <f>B1</f>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f>IF(L7&gt;=0,-1,1)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ref="B8:B38" si="0">DEGREES(ATAN(2^-A8))</f>
+        <v>26.56505117707799</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" ref="C8:C38" si="1">INT(B8/360*POWER(2,32))</f>
+        <v>316933405</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ref="D8:D38" si="2">SQRT(1+POWER(2, -2*A8))</f>
+        <v>1.1180339887498949</v>
+      </c>
+      <c r="F8" s="3">
+        <f>F7+(M7*INT(I7/(2^A7)))</f>
+        <v>-256</v>
+      </c>
+      <c r="G8" s="3" t="str">
+        <f t="shared" ref="G8:G38" si="3">DEC2HEX(F8,8)</f>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f t="shared" ref="H8:H38" si="4">DEC2HEX(F8/$B$3,8)</f>
+        <v>FFFFFFFF65</v>
+      </c>
+      <c r="I8" s="3">
+        <f>I7-(M7*INT(F7/(2^A7)))</f>
+        <v>-256</v>
+      </c>
+      <c r="J8" s="3" t="str">
+        <f t="shared" ref="J8:J38" si="5">DEC2HEX(I8,8)</f>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="K8" s="3" t="str">
+        <f t="shared" ref="K8:K38" si="6">DEC2HEX(I8/$B$3,8)</f>
+        <v>FFFFFFFF65</v>
+      </c>
+      <c r="L8" s="6">
+        <f>L7+C7*M7</f>
+        <v>-536870912</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:M38" si="7">IF(L8&gt;=0,-1,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>14.036243467926479</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>167458907</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0307764064044151</v>
+      </c>
+      <c r="F9" s="3">
+        <f>F8+(M8*INT(I8/(2^A8)))</f>
+        <v>-384</v>
+      </c>
+      <c r="G9" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE80</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF17</v>
+      </c>
+      <c r="I9" s="3">
+        <f>I8-(M8*INT(F8/(2^A8)))</f>
+        <v>-128</v>
+      </c>
+      <c r="J9" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFF80</v>
+      </c>
+      <c r="K9" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>FFFFFFFFB3</v>
+      </c>
+      <c r="L9" s="6">
+        <f>L8+C8*M8</f>
+        <v>-219937507</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>7.1250163489017977</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="1"/>
+        <v>85004756</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0077822185373186</v>
+      </c>
+      <c r="F10" s="3">
+        <f>F9+(M9*INT(I9/(2^A9)))</f>
+        <v>-416</v>
+      </c>
+      <c r="G10" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE60</v>
+      </c>
+      <c r="H10" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF04</v>
+      </c>
+      <c r="I10" s="3">
+        <f>I9-(M9*INT(F9/(2^A9)))</f>
+        <v>-32</v>
+      </c>
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFE0</v>
+      </c>
+      <c r="K10" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>FFFFFFFFED</v>
+      </c>
+      <c r="L10" s="6">
+        <f>L9+C9*M9</f>
+        <v>-52478600</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5763343749973511</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>42667331</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0019512213675874</v>
+      </c>
+      <c r="F11" s="3">
+        <f>F10+(M10*INT(I10/(2^A10)))</f>
+        <v>-420</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE5C</v>
+      </c>
+      <c r="H11" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF01</v>
+      </c>
+      <c r="I11" s="3">
+        <f>I10-(M10*INT(F10/(2^A10)))</f>
+        <v>20</v>
+      </c>
+      <c r="J11" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000014</v>
+      </c>
+      <c r="K11" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>0000000C</v>
+      </c>
+      <c r="L11" s="6">
+        <f>L10+C10*M10</f>
+        <v>32526156</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7899106082460694</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="1"/>
+        <v>21354465</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0004881620988826</v>
+      </c>
+      <c r="F12" s="3">
+        <f>F11+(M11*INT(I11/(2^A11)))</f>
+        <v>-421</v>
+      </c>
+      <c r="G12" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE5B</v>
+      </c>
+      <c r="H12" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF01</v>
+      </c>
+      <c r="I12" s="3">
+        <f>I11-(M11*INT(F11/(2^A11)))</f>
+        <v>-7</v>
+      </c>
+      <c r="J12" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFF9</v>
+      </c>
+      <c r="K12" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>FFFFFFFFFC</v>
+      </c>
+      <c r="L12" s="6">
+        <f>L11+C11*M11</f>
+        <v>-10141175</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.89517371021107439</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="1"/>
+        <v>10679838</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0001220628628287</v>
+      </c>
+      <c r="F13" s="3">
+        <f>F12+(M12*INT(I12/(2^A12)))</f>
+        <v>-422</v>
+      </c>
+      <c r="G13" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE5A</v>
+      </c>
+      <c r="H13" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="I13" s="3">
+        <f>I12-(M12*INT(F12/(2^A12)))</f>
+        <v>7</v>
+      </c>
+      <c r="J13" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000007</v>
+      </c>
+      <c r="K13" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000004</v>
+      </c>
+      <c r="L13" s="6">
+        <f>L12+C12*M12</f>
+        <v>11213290</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.44761417086055311</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>5340245</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000305171124779</v>
+      </c>
+      <c r="F14" s="3">
+        <f>F13+(M13*INT(I13/(2^A13)))</f>
+        <v>-422</v>
+      </c>
+      <c r="G14" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE5A</v>
+      </c>
+      <c r="H14" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="I14" s="3">
+        <f>I13-(M13*INT(F13/(2^A13)))</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K14" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L14" s="6">
+        <f>L13+C13*M13</f>
+        <v>533452</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.22381050036853808</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>2670163</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000076293654276</v>
+      </c>
+      <c r="F15" s="3">
+        <f>F14+(M14*INT(I14/(2^A14)))</f>
+        <v>-422</v>
+      </c>
+      <c r="G15" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE5A</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="I15" s="3">
+        <f>I14-(M14*INT(F14/(2^A14)))</f>
+        <v>-4</v>
+      </c>
+      <c r="J15" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFFC</v>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>FFFFFFFFFE</v>
+      </c>
+      <c r="L15" s="6">
+        <f>L14+C14*M14</f>
+        <v>-4806793</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1119056770662069</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="1"/>
+        <v>1335086</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000019073468138</v>
+      </c>
+      <c r="F16" s="3">
+        <f>F15+(M15*INT(I15/(2^A15)))</f>
+        <v>-423</v>
+      </c>
+      <c r="G16" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE59</v>
+      </c>
+      <c r="H16" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFF00</v>
+      </c>
+      <c r="I16" s="3">
+        <f>I15-(M15*INT(F15/(2^A15)))</f>
+        <v>-2</v>
+      </c>
+      <c r="J16" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFFE</v>
+      </c>
+      <c r="K16" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>FFFFFFFFFF</v>
+      </c>
+      <c r="L16" s="6">
+        <f>L15+C15*M15</f>
+        <v>-2136630</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>5.5952891893803675E-2</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>667544</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000004768370445</v>
+      </c>
+      <c r="F17" s="3">
+        <f>F16+(M16*INT(I16/(2^A16)))</f>
+        <v>-424</v>
+      </c>
+      <c r="G17" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE58</v>
+      </c>
+      <c r="H17" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFF</v>
+      </c>
+      <c r="I17" s="3">
+        <f>I16-(M16*INT(F16/(2^A16)))</f>
+        <v>-1</v>
+      </c>
+      <c r="J17" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFFF</v>
+      </c>
+      <c r="K17" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L17" s="6">
+        <f>L16+C16*M16</f>
+        <v>-801544</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7976452617003676E-2</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>333772</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000001192092824</v>
+      </c>
+      <c r="F18" s="3">
+        <f>F17+(M17*INT(I17/(2^A17)))</f>
+        <v>-425</v>
+      </c>
+      <c r="G18" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE57</v>
+      </c>
+      <c r="H18" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I18" s="3">
+        <f>I17-(M17*INT(F17/(2^A17)))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K18" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L18" s="6">
+        <f>L17+C17*M17</f>
+        <v>-134000</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3988227142265016E-2</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>166886</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000298023219</v>
+      </c>
+      <c r="F19" s="3">
+        <f>F18+(M18*INT(I18/(2^A18)))</f>
+        <v>-425</v>
+      </c>
+      <c r="G19" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE57</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I19" s="3">
+        <f>I18-(M18*INT(F18/(2^A18)))</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K19" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L19" s="6">
+        <f>L18+C18*M18</f>
+        <v>199772</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9941136753529191E-3</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>83443</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000074505806</v>
+      </c>
+      <c r="F20" s="3">
+        <f>F19+(M19*INT(I19/(2^A19)))</f>
+        <v>-425</v>
+      </c>
+      <c r="G20" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE57</v>
+      </c>
+      <c r="H20" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I20" s="3">
+        <f>I19-(M19*INT(F19/(2^A19)))</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K20" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L20" s="6">
+        <f>L19+C19*M19</f>
+        <v>32886</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4970568507040108E-3</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>41721</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000018626451</v>
+      </c>
+      <c r="F21" s="3">
+        <f>F20+(M20*INT(I20/(2^A20)))</f>
+        <v>-425</v>
+      </c>
+      <c r="G21" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE57</v>
+      </c>
+      <c r="H21" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I21" s="3">
+        <f>I20-(M20*INT(F20/(2^A20)))</f>
+        <v>-1</v>
+      </c>
+      <c r="J21" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFFF</v>
+      </c>
+      <c r="K21" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L21" s="6">
+        <f>L20+C20*M20</f>
+        <v>-50557</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7485284269804495E-3</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>20860</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000004656613</v>
+      </c>
+      <c r="F22" s="3">
+        <f>F21+(M21*INT(I21/(2^A21)))</f>
+        <v>-426</v>
+      </c>
+      <c r="G22" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE56</v>
+      </c>
+      <c r="H22" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I22" s="3">
+        <f>I21-(M21*INT(F21/(2^A21)))</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K22" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L22" s="6">
+        <f>L21+C21*M21</f>
+        <v>-8836</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>8.7426421369378026E-4</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>10430</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000001164153</v>
+      </c>
+      <c r="F23" s="3">
+        <f>F22+(M22*INT(I22/(2^A22)))</f>
+        <v>-426</v>
+      </c>
+      <c r="G23" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE56</v>
+      </c>
+      <c r="H23" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I23" s="3">
+        <f>I22-(M22*INT(F22/(2^A22)))</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K23" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L23" s="6">
+        <f>L22+C22*M22</f>
+        <v>12024</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="0"/>
+        <v>4.3713210687233457E-4</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="1"/>
+        <v>5215</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000291038</v>
+      </c>
+      <c r="F24" s="3">
+        <f>F23+(M23*INT(I23/(2^A23)))</f>
+        <v>-426</v>
+      </c>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE56</v>
+      </c>
+      <c r="H24" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I24" s="3">
+        <f>I23-(M23*INT(F23/(2^A23)))</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K24" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L24" s="6">
+        <f>L23+C23*M23</f>
+        <v>1594</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1856605343934784E-4</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="1"/>
+        <v>2607</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="2"/>
+        <v>1.000000000007276</v>
+      </c>
+      <c r="F25" s="3">
+        <f>F24+(M24*INT(I24/(2^A24)))</f>
+        <v>-426</v>
+      </c>
+      <c r="G25" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE56</v>
+      </c>
+      <c r="H25" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFE</v>
+      </c>
+      <c r="I25" s="3">
+        <f>I24-(M24*INT(F24/(2^A24)))</f>
+        <v>-1</v>
+      </c>
+      <c r="J25" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFFF</v>
+      </c>
+      <c r="K25" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L25" s="6">
+        <f>L24+C24*M24</f>
+        <v>-3621</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0928302672007149E-4</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="1"/>
+        <v>1303</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="2"/>
+        <v>1.000000000001819</v>
+      </c>
+      <c r="F26" s="3">
+        <f>F25+(M25*INT(I25/(2^A25)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H26" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I26" s="3">
+        <f>I25-(M25*INT(F25/(2^A25)))</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K26" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L26" s="6">
+        <f>L25+C25*M25</f>
+        <v>-1014</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="0"/>
+        <v>5.464151336008544E-5</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="1"/>
+        <v>651</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000004547</v>
+      </c>
+      <c r="F27" s="3">
+        <f>F26+(M26*INT(I26/(2^A26)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H27" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I27" s="3">
+        <f>I26-(M26*INT(F26/(2^A26)))</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K27" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L27" s="6">
+        <f>L26+C26*M26</f>
+        <v>289</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7320756680048934E-5</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="1"/>
+        <v>325</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000001137</v>
+      </c>
+      <c r="F28" s="3">
+        <f>F27+(M27*INT(I27/(2^A27)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G28" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H28" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I28" s="3">
+        <f>I27-(M27*INT(F27/(2^A27)))</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K28" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L28" s="6">
+        <f>L27+C27*M27</f>
+        <v>-362</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3660378340025243E-5</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000284</v>
+      </c>
+      <c r="F29" s="3">
+        <f>F28+(M28*INT(I28/(2^A28)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H29" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I29" s="3">
+        <f>I28-(M28*INT(F28/(2^A28)))</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K29" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L29" s="6">
+        <f>L28+C28*M28</f>
+        <v>-37</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>6.8301891700127188E-6</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000071</v>
+      </c>
+      <c r="F30" s="3">
+        <f>F29+(M29*INT(I29/(2^A29)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H30" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I30" s="3">
+        <f>I29-(M29*INT(F29/(2^A29)))</f>
+        <v>2</v>
+      </c>
+      <c r="J30" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000002</v>
+      </c>
+      <c r="K30" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000001</v>
+      </c>
+      <c r="L30" s="6">
+        <f>L29+C29*M29</f>
+        <v>125</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4150945850063712E-6</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000018</v>
+      </c>
+      <c r="F31" s="3">
+        <f>F30+(M30*INT(I30/(2^A30)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G31" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H31" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I31" s="3">
+        <f>I30-(M30*INT(F30/(2^A30)))</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K31" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L31" s="6">
+        <f>L30+C30*M30</f>
+        <v>44</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7075472925031871E-6</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="F32" s="3">
+        <f>F31+(M31*INT(I31/(2^A31)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H32" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I32" s="3">
+        <f>I31-(M31*INT(F31/(2^A31)))</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K32" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L32" s="6">
+        <f>L31+C31*M31</f>
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5377364625159377E-7</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <f>F32+(M32*INT(I32/(2^A32)))</f>
+        <v>-427</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE55</v>
+      </c>
+      <c r="H33" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I33" s="3">
+        <f>I32-(M32*INT(F32/(2^A32)))</f>
+        <v>-1</v>
+      </c>
+      <c r="J33" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>FFFFFFFFFF</v>
+      </c>
+      <c r="K33" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L33" s="6">
+        <f>L32+C32*M32</f>
+        <v>-16</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34">
+        <v>27</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2688682312579694E-7</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <f>F33+(M33*INT(I33/(2^A33)))</f>
+        <v>-428</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE54</v>
+      </c>
+      <c r="H34" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I34" s="3">
+        <f>I33-(M33*INT(F33/(2^A33)))</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K34" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L34" s="6">
+        <f>L33+C33*M33</f>
+        <v>-6</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35">
+        <v>28</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1344341156289847E-7</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="3">
+        <f>F34+(M34*INT(I34/(2^A34)))</f>
+        <v>-428</v>
+      </c>
+      <c r="G35" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE54</v>
+      </c>
+      <c r="H35" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I35" s="3">
+        <f>I34-(M34*INT(F34/(2^A34)))</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K35" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L35" s="6">
+        <f>L34+C34*M34</f>
+        <v>-1</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36">
+        <v>29</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0672170578144923E-7</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <f>F35+(M35*INT(I35/(2^A35)))</f>
+        <v>-428</v>
+      </c>
+      <c r="G36" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE54</v>
+      </c>
+      <c r="H36" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I36" s="3">
+        <f>I35-(M35*INT(F35/(2^A35)))</f>
+        <v>2</v>
+      </c>
+      <c r="J36" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000002</v>
+      </c>
+      <c r="K36" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000001</v>
+      </c>
+      <c r="L36" s="6">
+        <f>L35+C35*M35</f>
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3360852890724617E-8</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="3">
+        <f>F36+(M36*INT(I36/(2^A36)))</f>
+        <v>-428</v>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE54</v>
+      </c>
+      <c r="H37" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I37" s="3">
+        <f>I36-(M36*INT(F36/(2^A36)))</f>
+        <v>1</v>
+      </c>
+      <c r="J37" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000001</v>
+      </c>
+      <c r="K37" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L37" s="6">
+        <f>L36+C36*M36</f>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="0"/>
+        <v>2.6680426445362308E-8</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <f>F37+(M37*INT(I37/(2^A37)))</f>
+        <v>-428</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>FFFFFFFE54</v>
+      </c>
+      <c r="H38" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>FFFFFFFEFD</v>
+      </c>
+      <c r="I38" s="3">
+        <f>I37-(M37*INT(F37/(2^A37)))</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="K38" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+      <c r="L38" s="6">
+        <f>L37+C37*M37</f>
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3490,11 +5177,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -5372,4 +7061,1127 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:D68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D68" sqref="A68:D68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <f>DEGREES(ATAN(2^-A4))</f>
+        <v>45</v>
+      </c>
+      <c r="C4" s="7">
+        <f>B4/360*POWER(2,64)</f>
+        <v>2.305843009213694E+18</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>DEC2HEX(INT(B4/360*POWER(2,32)),8)</f>
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ref="B5:B35" si="0">DEGREES(ATAN(2^-A5))</f>
+        <v>26.56505117707799</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" ref="C5:C68" si="1">B5/360*POWER(2,64)</f>
+        <v>1.3612186121348733E+18</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" ref="D5:D35" si="2">DEC2HEX(INT(B5/360*POWER(2,32)),8)</f>
+        <v>12E4051D</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>14.036243467926479</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="1"/>
+        <v>7.1923053058088102E+17</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>09FB385B</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>7.1250163489017977</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="1"/>
+        <v>3.6509264752552198E+17</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>051111D4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5763343749973511</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="1"/>
+        <v>1.8325479149329482E+17</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>028B0D43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7899106082460694</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="1"/>
+        <v>9.1716730292036224E+16</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0145D7E1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.89517371021107439</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="1"/>
+        <v>4.5869556482713136E+16</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00A2F61E</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.44761417086055311</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="1"/>
+        <v>2.2936177926750896E+16</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00517C55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.22381050036853808</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1468263948075832E+16</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0028BE53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1119056770662069</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="1"/>
+        <v>5734153847876408</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00145F2E</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5.5952891893803675E-2</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="1"/>
+        <v>2867079658191483.5</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>000A2F98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7976452617003676E-2</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="1"/>
+        <v>1433540170878135</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>000517CC</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3988227142265016E-2</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="1"/>
+        <v>716770128161889.75</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00028BE6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9941136753529191E-3</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>358385069421298.31</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>000145F3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4970568507040108E-3</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>179192535378193.34</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0000A2F9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7485284269804495E-3</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>89596267772539.703</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0000517C</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>8.7426421369378026E-4</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>44798133896700.227</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>000028BE</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>4.3713210687233457E-4</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>22399066949653.91</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0000145F</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1856605343934784E-4</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>11199533474989.93</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000A2F</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0928302672007149E-4</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="1"/>
+        <v>5599766737515.3369</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="0"/>
+        <v>5.464151336008544E-5</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="1"/>
+        <v>2799883368760.2148</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0000028B</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7320756680048934E-5</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="1"/>
+        <v>1399941684380.4258</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3660378340025243E-5</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="1"/>
+        <v>699970842190.25269</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>000000A2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="0"/>
+        <v>6.8301891700127188E-6</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="1"/>
+        <v>349985421095.13135</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000051</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4150945850063712E-6</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="1"/>
+        <v>174992710547.56628</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000028</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7075472925031871E-6</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="1"/>
+        <v>87496355273.783218</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5377364625159377E-7</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="1"/>
+        <v>43748177636.891617</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2688682312579694E-7</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="1"/>
+        <v>21874088818.445812</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1344341156289847E-7</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="1"/>
+        <v>10937044409.222906</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0672170578144923E-7</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="1"/>
+        <v>5468522204.6114531</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3360852890724617E-8</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>2734261102.3057265</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="0"/>
+        <v>2.6680426445362308E-8</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
+        <v>1367130551.1528633</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" ref="B36:B68" si="3">DEGREES(ATAN(2^-A36))</f>
+        <v>1.3340213222681154E-8</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="1"/>
+        <v>683565275.57643163</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" ref="D36:D68" si="4">DEC2HEX(INT(B36/360*POWER(2,32)),8)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="3"/>
+        <v>6.6701066113405771E-9</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="1"/>
+        <v>341782637.78821582</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="3"/>
+        <v>3.3350533056702886E-9</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="1"/>
+        <v>170891318.89410791</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6675266528351443E-9</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="1"/>
+        <v>85445659.447053954</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3376332641757214E-10</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="1"/>
+        <v>42722829.723526977</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="3"/>
+        <v>4.1688166320878607E-10</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="1"/>
+        <v>21361414.861763489</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="3"/>
+        <v>2.0844083160439303E-10</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="1"/>
+        <v>10680707.430881744</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0422041580219652E-10</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="1"/>
+        <v>5340353.7154408721</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44" s="3">
+        <f t="shared" si="3"/>
+        <v>5.2110207901098259E-11</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="1"/>
+        <v>2670176.8577204361</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="3"/>
+        <v>2.6055103950549129E-11</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="1"/>
+        <v>1335088.428860218</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3027551975274565E-11</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="1"/>
+        <v>667544.21443010902</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47" s="3">
+        <f t="shared" si="3"/>
+        <v>6.5137759876372823E-12</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="1"/>
+        <v>333772.10721505451</v>
+      </c>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48" s="3">
+        <f t="shared" si="3"/>
+        <v>3.2568879938186412E-12</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="1"/>
+        <v>166886.05360752725</v>
+      </c>
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6284439969093206E-12</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="1"/>
+        <v>83443.026803763627</v>
+      </c>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50" s="3">
+        <f t="shared" si="3"/>
+        <v>8.1422199845466029E-13</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="1"/>
+        <v>41721.513401881813</v>
+      </c>
+      <c r="D50" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51" s="3">
+        <f t="shared" si="3"/>
+        <v>4.0711099922733015E-13</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="1"/>
+        <v>20860.756700940907</v>
+      </c>
+      <c r="D51" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" si="3"/>
+        <v>2.0355549961366507E-13</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="1"/>
+        <v>10430.378350470453</v>
+      </c>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0177774980683254E-13</v>
+      </c>
+      <c r="C53" s="6">
+        <f t="shared" si="1"/>
+        <v>5215.1891752352267</v>
+      </c>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0888874903416268E-14</v>
+      </c>
+      <c r="C54" s="6">
+        <f t="shared" si="1"/>
+        <v>2607.5945876176133</v>
+      </c>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55" s="3">
+        <f t="shared" si="3"/>
+        <v>2.5444437451708134E-14</v>
+      </c>
+      <c r="C55" s="6">
+        <f t="shared" si="1"/>
+        <v>1303.7972938088067</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="B56" s="3">
+        <f t="shared" si="3"/>
+        <v>1.2722218725854067E-14</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="1"/>
+        <v>651.89864690440334</v>
+      </c>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>53</v>
+      </c>
+      <c r="B57" s="3">
+        <f t="shared" si="3"/>
+        <v>6.3611093629270335E-15</v>
+      </c>
+      <c r="C57" s="6">
+        <f t="shared" si="1"/>
+        <v>325.94932345220167</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>54</v>
+      </c>
+      <c r="B58" s="3">
+        <f t="shared" si="3"/>
+        <v>3.1805546814635168E-15</v>
+      </c>
+      <c r="C58" s="6">
+        <f t="shared" si="1"/>
+        <v>162.97466172610083</v>
+      </c>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>55</v>
+      </c>
+      <c r="B59" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5902773407317584E-15</v>
+      </c>
+      <c r="C59" s="6">
+        <f t="shared" si="1"/>
+        <v>81.487330863050417</v>
+      </c>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>56</v>
+      </c>
+      <c r="B60" s="3">
+        <f t="shared" si="3"/>
+        <v>7.9513867036587919E-16</v>
+      </c>
+      <c r="C60" s="6">
+        <f t="shared" si="1"/>
+        <v>40.743665431525208</v>
+      </c>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>57</v>
+      </c>
+      <c r="B61" s="3">
+        <f t="shared" si="3"/>
+        <v>3.975693351829396E-16</v>
+      </c>
+      <c r="C61" s="6">
+        <f t="shared" si="1"/>
+        <v>20.371832715762604</v>
+      </c>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>58</v>
+      </c>
+      <c r="B62" s="3">
+        <f t="shared" si="3"/>
+        <v>1.987846675914698E-16</v>
+      </c>
+      <c r="C62" s="6">
+        <f t="shared" si="1"/>
+        <v>10.185916357881302</v>
+      </c>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>59</v>
+      </c>
+      <c r="B63" s="3">
+        <f t="shared" si="3"/>
+        <v>9.9392333795734899E-17</v>
+      </c>
+      <c r="C63" s="6">
+        <f t="shared" si="1"/>
+        <v>5.0929581789406511</v>
+      </c>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>60</v>
+      </c>
+      <c r="B64" s="3">
+        <f t="shared" si="3"/>
+        <v>4.9696166897867449E-17</v>
+      </c>
+      <c r="C64" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5464790894703255</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>61</v>
+      </c>
+      <c r="B65" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4848083448933725E-17</v>
+      </c>
+      <c r="C65" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2732395447351628</v>
+      </c>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>62</v>
+      </c>
+      <c r="B66" s="3">
+        <f t="shared" si="3"/>
+        <v>1.2424041724466862E-17</v>
+      </c>
+      <c r="C66" s="6">
+        <f t="shared" si="1"/>
+        <v>0.63661977236758138</v>
+      </c>
+      <c r="D66" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>63</v>
+      </c>
+      <c r="B67" s="3">
+        <f t="shared" si="3"/>
+        <v>6.2120208622334312E-18</v>
+      </c>
+      <c r="C67" s="6">
+        <f t="shared" si="1"/>
+        <v>0.31830988618379069</v>
+      </c>
+      <c r="D67" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="B68" s="3"/>
+      <c r="D68" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>